<commit_message>
Use FT instead of INF
</commit_message>
<xml_diff>
--- a/VT_IE_AGR.xlsx
+++ b/VT_IE_AGR.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044FBACC-3398-4311-B971-49315BB4D4F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56CCC98-F7FD-4987-A69A-B16BBC7A6AAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="30" r:id="rId1"/>
@@ -51346,8 +51346,8 @@
   </sheetPr>
   <dimension ref="B3:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -52575,8 +52575,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52675,7 +52675,7 @@
       </c>
       <c r="C5" s="554" t="str">
         <f>M5</f>
-        <v>AGRBGS_INF</v>
+        <v>FT-AGRBGS</v>
       </c>
       <c r="D5" s="559" t="s">
         <v>560</v>
@@ -52700,8 +52700,8 @@
         <v>IE,National</v>
       </c>
       <c r="M5" s="554" t="str">
-        <f>Commodities!D40&amp;"_INF"</f>
-        <v>AGRBGS_INF</v>
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D40)</f>
+        <v>FT-AGRBGS</v>
       </c>
       <c r="N5" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E40</f>
@@ -52729,9 +52729,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M6" s="554" t="str">
-        <f>Commodities!D41&amp;"_INF"</f>
-        <v>AGRBDL_INF</v>
+      <c r="M6" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D41)</f>
+        <v>FT-AGRBDL</v>
       </c>
       <c r="N6" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E41</f>
@@ -52751,7 +52751,7 @@
       </c>
       <c r="C7" s="554" t="str">
         <f>M6</f>
-        <v>AGRBDL_INF</v>
+        <v>FT-AGRBDL</v>
       </c>
       <c r="D7" s="554" t="s">
         <v>550</v>
@@ -52772,9 +52772,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M7" s="554" t="str">
-        <f>Commodities!D42&amp;"_INF"</f>
-        <v>AGRBIO_INF</v>
+      <c r="M7" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D42)</f>
+        <v>FT-AGRBIO</v>
       </c>
       <c r="N7" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E42</f>
@@ -52795,9 +52795,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M8" s="554" t="str">
-        <f>Commodities!D43&amp;"_INF"</f>
-        <v>AGRDST_INF</v>
+      <c r="M8" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D43)</f>
+        <v>FT-AGRDST</v>
       </c>
       <c r="N8" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E43</f>
@@ -52817,7 +52817,7 @@
       </c>
       <c r="C9" s="554" t="str">
         <f>M7</f>
-        <v>AGRBIO_INF</v>
+        <v>FT-AGRBIO</v>
       </c>
       <c r="D9" s="561" t="s">
         <v>566</v>
@@ -52838,9 +52838,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M9" s="554" t="str">
-        <f>Commodities!D44&amp;"_INF"</f>
-        <v>AGRELC_INF</v>
+      <c r="M9" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D44)</f>
+        <v>FT-AGRELC</v>
       </c>
       <c r="N9" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E44</f>
@@ -52868,9 +52868,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M10" s="554" t="str">
-        <f>Commodities!D45&amp;"_INF"</f>
-        <v>AGRGAS_INF</v>
+      <c r="M10" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D45)</f>
+        <v>FT-AGRGAS</v>
       </c>
       <c r="N10" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E45</f>
@@ -52893,7 +52893,7 @@
       </c>
       <c r="C11" s="554" t="str">
         <f t="shared" si="0"/>
-        <v>AGRDST_INF</v>
+        <v>FT-AGRDST</v>
       </c>
       <c r="D11" s="559" t="s">
         <v>549</v>
@@ -52914,9 +52914,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M11" s="554" t="str">
-        <f>Commodities!D46&amp;"_INF"</f>
-        <v>AGRGEO_INF</v>
+      <c r="M11" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D46)</f>
+        <v>FT-AGRGEO</v>
       </c>
       <c r="N11" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E46</f>
@@ -52936,7 +52936,7 @@
       </c>
       <c r="C12" s="554" t="str">
         <f t="shared" si="0"/>
-        <v>AGRELC_INF</v>
+        <v>FT-AGRELC</v>
       </c>
       <c r="D12" s="562" t="s">
         <v>552</v>
@@ -52957,9 +52957,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M12" s="554" t="str">
-        <f>Commodities!D47&amp;"_INF"</f>
-        <v>AGRHET_INF</v>
+      <c r="M12" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D47)</f>
+        <v>FT-AGRHET</v>
       </c>
       <c r="N12" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E47</f>
@@ -52979,7 +52979,7 @@
       </c>
       <c r="C13" s="554" t="str">
         <f t="shared" si="0"/>
-        <v>AGRGAS_INF</v>
+        <v>FT-AGRGAS</v>
       </c>
       <c r="D13" s="559" t="s">
         <v>553</v>
@@ -53000,9 +53000,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M13" s="554" t="str">
-        <f>Commodities!D48&amp;"_INF"</f>
-        <v>AGRLPG_INF</v>
+      <c r="M13" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D48)</f>
+        <v>FT-AGRLPG</v>
       </c>
       <c r="N13" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E48</f>
@@ -53022,7 +53022,7 @@
       </c>
       <c r="C14" s="554" t="str">
         <f t="shared" si="0"/>
-        <v>AGRGEO_INF</v>
+        <v>FT-AGRGEO</v>
       </c>
       <c r="D14" s="563" t="s">
         <v>554</v>
@@ -53043,9 +53043,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M14" s="554" t="str">
-        <f>Commodities!D49&amp;"_INF"</f>
-        <v>AGRSOL_INF</v>
+      <c r="M14" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D49)</f>
+        <v>FT-AGRSOL</v>
       </c>
       <c r="N14" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E49</f>
@@ -53065,7 +53065,7 @@
       </c>
       <c r="C15" s="554" t="str">
         <f t="shared" si="1"/>
-        <v>AGRHET_INF</v>
+        <v>FT-AGRHET</v>
       </c>
       <c r="D15" s="554" t="s">
         <v>605</v>
@@ -53086,9 +53086,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M15" s="554" t="str">
-        <f>Commodities!D50&amp;"_INF"</f>
-        <v>AGRH2G_INF</v>
+      <c r="M15" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D50)</f>
+        <v>FT-AGRH2G</v>
       </c>
       <c r="N15" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E50</f>
@@ -53111,7 +53111,7 @@
       </c>
       <c r="C16" s="554" t="str">
         <f t="shared" si="1"/>
-        <v>AGRLPG_INF</v>
+        <v>FT-AGRLPG</v>
       </c>
       <c r="D16" s="559" t="s">
         <v>555</v>
@@ -53132,9 +53132,9 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="M16" s="554" t="str">
-        <f>Commodities!D51&amp;"_INF"</f>
-        <v>AGRH2L_INF</v>
+      <c r="M16" s="559" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,"FT",Commodities!D51)</f>
+        <v>FT-AGRH2L</v>
       </c>
       <c r="N16" s="554" t="str">
         <f>"Fuel tech - "&amp;Commodities!E51</f>
@@ -53157,7 +53157,7 @@
       </c>
       <c r="C17" s="554" t="str">
         <f t="shared" si="1"/>
-        <v>AGRSOL_INF</v>
+        <v>FT-AGRSOL</v>
       </c>
       <c r="D17" s="559" t="s">
         <v>556</v>
@@ -53180,7 +53180,7 @@
       </c>
       <c r="C18" s="554" t="str">
         <f t="shared" si="1"/>
-        <v>AGRH2G_INF</v>
+        <v>FT-AGRH2G</v>
       </c>
       <c r="D18" s="565" t="s">
         <v>611</v>
@@ -53203,7 +53203,7 @@
       </c>
       <c r="C19" s="554" t="str">
         <f t="shared" si="1"/>
-        <v>AGRH2L_INF</v>
+        <v>FT-AGRH2L</v>
       </c>
       <c r="D19" s="565" t="s">
         <v>612</v>

</xml_diff>

<commit_message>
Use DayNite for ELC and HET FTs, remove Season and update units
</commit_message>
<xml_diff>
--- a/VT_IE_AGR.xlsx
+++ b/VT_IE_AGR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEF44C9-94C4-4415-8016-4E46E268F8C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC29D656-3ECB-4A19-A3EC-6654420FFE21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="30" r:id="rId1"/>
@@ -1860,7 +1860,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="685">
   <si>
     <t>~FI_T</t>
   </si>
@@ -3999,10 +3999,17 @@
     <numFmt numFmtId="170" formatCode="0E+00"/>
     <numFmt numFmtId="171" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4618,22 +4625,22 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="580">
+  <cellXfs count="581">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4648,10 +4655,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -4659,8 +4666,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4669,7 +4676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -4717,139 +4724,139 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -4858,226 +4865,226 @@
     <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -5101,13 +5108,13 @@
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -5155,70 +5162,70 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -5236,71 +5243,71 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5309,660 +5316,660 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="15" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="15" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="28" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="27" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -5971,152 +5978,237 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6124,102 +6216,14 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6228,70 +6232,76 @@
     <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="32" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="33" fillId="15" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -52584,8 +52594,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52722,9 +52732,7 @@
       <c r="P5" s="554" t="s">
         <v>274</v>
       </c>
-      <c r="Q5" s="564" t="s">
-        <v>569</v>
-      </c>
+      <c r="Q5" s="564"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="D6" s="559" t="s">
@@ -52891,9 +52899,7 @@
       <c r="P10" s="554" t="s">
         <v>274</v>
       </c>
-      <c r="Q10" s="564" t="s">
-        <v>569</v>
-      </c>
+      <c r="Q10" s="564"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" s="559" t="str">
@@ -52980,6 +52986,9 @@
       <c r="P12" s="554" t="s">
         <v>274</v>
       </c>
+      <c r="Q12" s="580" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="559" t="str">
@@ -53109,9 +53118,7 @@
       <c r="P15" s="554" t="s">
         <v>274</v>
       </c>
-      <c r="Q15" s="564" t="s">
-        <v>569</v>
-      </c>
+      <c r="Q15" s="564"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" s="559" t="str">
@@ -53155,9 +53162,7 @@
       <c r="P16" s="554" t="s">
         <v>274</v>
       </c>
-      <c r="Q16" s="564" t="s">
-        <v>569</v>
-      </c>
+      <c r="Q16" s="564"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="559" t="str">
@@ -63261,7 +63266,7 @@
   </sheetPr>
   <dimension ref="B3:AH71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>

</xml_diff>